<commit_message>
Trying my own single function
</commit_message>
<xml_diff>
--- a/CH-127 Add Index Column.xlsx
+++ b/CH-127 Add Index Column.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80425F0A-D70B-4E91-9923-9758E7046166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB060C9-4614-4E74-8C8A-AD9B8532B601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,16 @@
     <sheet name="Alt2" sheetId="3" r:id="rId3"/>
     <sheet name="Alt3" sheetId="4" r:id="rId4"/>
     <sheet name="EDA" sheetId="5" r:id="rId5"/>
+    <sheet name="EDA2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$E$2:$G$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$E$2:$G$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt3'!$E$2:$G$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">EDA!$E$2:$G$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'EDA2'!$E$2:$G$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$E$2:$G$15</definedName>
+    <definedName name="_nC" localSheetId="5">'EDA2'!$B$17</definedName>
     <definedName name="_nC">EDA!$B$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -70,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="11">
   <si>
     <t>Result</t>
   </si>
@@ -160,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -329,6 +338,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -755,7 +765,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="918" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="525" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1469,7 +1479,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2516,8 +2526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED11655-21B6-4857-A475-05D6E876A63B}">
   <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2830,14 +2840,14 @@
       <c r="V17">
         <v>1</v>
       </c>
-      <c r="X17" t="str" cm="1">
+      <c r="X17" s="14" t="str" cm="1">
         <f t="array" ref="X17:Z27">_xlfn.DROP(_xlfn._xlws.SORT(_xlfn.ANCHORARRAY(S17),4),,-1)</f>
         <v>A</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="14">
         <v>100</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="14">
         <v>1</v>
       </c>
       <c r="AB17" t="b" cm="1">
@@ -2897,13 +2907,13 @@
       <c r="V18">
         <v>2</v>
       </c>
-      <c r="X18" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y18">
+      <c r="X18" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y18" s="14">
         <v>45</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="14">
         <v>1</v>
       </c>
       <c r="AB18" t="b">
@@ -2962,13 +2972,13 @@
       <c r="V19">
         <v>3</v>
       </c>
-      <c r="X19" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y19">
+      <c r="X19" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y19" s="14">
         <v>88</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="14">
         <v>2</v>
       </c>
       <c r="AB19" t="b">
@@ -3027,13 +3037,13 @@
       <c r="V20">
         <v>6</v>
       </c>
-      <c r="X20" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y20">
+      <c r="X20" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y20" s="14">
         <v>49</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="14">
         <v>1</v>
       </c>
       <c r="AB20" t="b">
@@ -3092,13 +3102,13 @@
       <c r="V21">
         <v>8</v>
       </c>
-      <c r="X21" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y21">
+      <c r="X21" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y21" s="14">
         <v>43</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="14">
         <v>1</v>
       </c>
       <c r="AB21" t="b">
@@ -3145,13 +3155,13 @@
       <c r="V22">
         <v>9</v>
       </c>
-      <c r="X22" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y22">
+      <c r="X22" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y22" s="14">
         <v>96</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="14">
         <v>3</v>
       </c>
       <c r="AB22" t="b">
@@ -3195,13 +3205,13 @@
       <c r="V23">
         <v>4</v>
       </c>
-      <c r="X23" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y23">
+      <c r="X23" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y23" s="14">
         <v>84</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="14">
         <v>2</v>
       </c>
       <c r="AB23" t="b">
@@ -3266,13 +3276,13 @@
       <c r="V24">
         <v>5</v>
       </c>
-      <c r="X24" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y24">
+      <c r="X24" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y24" s="14">
         <v>99</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="14">
         <v>4</v>
       </c>
       <c r="AB24" t="b">
@@ -3331,13 +3341,13 @@
       <c r="V25">
         <v>7</v>
       </c>
-      <c r="X25" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y25">
+      <c r="X25" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y25" s="14">
         <v>69</v>
       </c>
-      <c r="Z25">
+      <c r="Z25" s="14">
         <v>1</v>
       </c>
       <c r="AB25" t="b">
@@ -3396,13 +3406,13 @@
       <c r="V26">
         <v>10</v>
       </c>
-      <c r="X26" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y26">
+      <c r="X26" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y26" s="14">
         <v>14</v>
       </c>
-      <c r="Z26">
+      <c r="Z26" s="14">
         <v>1</v>
       </c>
       <c r="AB26" t="b">
@@ -3461,13 +3471,13 @@
       <c r="V27">
         <v>11</v>
       </c>
-      <c r="X27" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y27">
+      <c r="X27" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y27" s="14">
         <v>22</v>
       </c>
-      <c r="Z27">
+      <c r="Z27" s="14">
         <v>2</v>
       </c>
       <c r="AB27" t="b">
@@ -3496,6 +3506,1171 @@
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0759260A-3526-4E7B-9B81-CFE36C329450}">
+  <dimension ref="A1:AD42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="E1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7">
+        <v>100</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>100</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <v>45</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>45</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <v>88</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>88</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>49</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="9">
+        <v>49</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <v>43</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="9">
+        <v>43</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7">
+        <v>96</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9">
+        <v>96</v>
+      </c>
+      <c r="G8" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7">
+        <v>84</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="9">
+        <v>84</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7">
+        <v>99</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="9">
+        <v>99</v>
+      </c>
+      <c r="G10" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="9">
+        <v>69</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="9">
+        <v>14</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="9">
+        <v>22</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f>COUNTA(B3:B13)</f>
+        <v>11</v>
+      </c>
+      <c r="C17" t="str" cm="1">
+        <f t="array" ref="C17:E27">_xlfn.HSTACK(B3:C13,_xlfn.SEQUENCE(_nC))</f>
+        <v>A</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="str" cm="1">
+        <f t="array" ref="G17:I22">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY($C$17),_xlfn.TAKE(_xlfn.ANCHORARRAY($C$17),,1)=H16)</f>
+        <v>A</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="K17" cm="1">
+        <f t="array" ref="K17:K21">_xlfn.DROP(_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(G17),2),-1)</f>
+        <v>100</v>
+      </c>
+      <c r="L17" cm="1">
+        <f t="array" ref="L17:L21">_xlfn.DROP(_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(G17),2),1)</f>
+        <v>45</v>
+      </c>
+      <c r="M17" cm="1">
+        <f t="array" ref="M17:M21">IF(_xlfn.ANCHORARRAY(K17)&gt;_xlfn.ANCHORARRAY(L17),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" cm="1">
+        <f t="array" ref="N17:N21">_xlfn.SCAN(0,_xlfn.ANCHORARRAY(M17),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v=0,1,_xlpm.a+1)))</f>
+        <v>1</v>
+      </c>
+      <c r="P17" cm="1">
+        <f t="array" ref="P17:P22">_xlfn.VSTACK(1,_xlfn.ANCHORARRAY(N17))</f>
+        <v>1</v>
+      </c>
+      <c r="S17" t="str" cm="1">
+        <f t="array" ref="S17:V27">_xlfn.VSTACK(_xlfn.HSTACK(G17:G22,H17:H22,_xlfn.ANCHORARRAY(P17),I17:I22),_xlfn.HSTACK(G24:G28,H24:H28,_xlfn.ANCHORARRAY(P24),I24:I28))</f>
+        <v>A</v>
+      </c>
+      <c r="T17">
+        <v>100</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="X17" s="14" t="str" cm="1">
+        <f t="array" ref="X17:Z27">_xlfn.DROP(_xlfn._xlws.SORT(_xlfn.ANCHORARRAY(S17),4),,-1)</f>
+        <v>A</v>
+      </c>
+      <c r="Y17" s="14">
+        <v>100</v>
+      </c>
+      <c r="Z17" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="b" cm="1">
+        <f t="array" ref="AB17:AD27">E3:G13=_xlfn.ANCHORARRAY(X17)</f>
+        <v>1</v>
+      </c>
+      <c r="AC17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C18" t="str">
+        <v>A</v>
+      </c>
+      <c r="D18">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="str">
+        <v>A</v>
+      </c>
+      <c r="H18">
+        <v>45</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>45</v>
+      </c>
+      <c r="L18">
+        <v>88</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="S18" t="str">
+        <v>A</v>
+      </c>
+      <c r="T18">
+        <v>45</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>2</v>
+      </c>
+      <c r="X18" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y18" s="14">
+        <v>45</v>
+      </c>
+      <c r="Z18" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C19" t="str">
+        <v>A</v>
+      </c>
+      <c r="D19">
+        <v>88</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="G19" t="str">
+        <v>A</v>
+      </c>
+      <c r="H19">
+        <v>88</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>88</v>
+      </c>
+      <c r="L19">
+        <v>96</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+      <c r="S19" t="str">
+        <v>A</v>
+      </c>
+      <c r="T19">
+        <v>88</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <v>3</v>
+      </c>
+      <c r="X19" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y19" s="14">
+        <v>88</v>
+      </c>
+      <c r="Z19" s="14">
+        <v>2</v>
+      </c>
+      <c r="AB19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C20" t="str">
+        <v>B</v>
+      </c>
+      <c r="D20">
+        <v>49</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="G20" t="str">
+        <v>A</v>
+      </c>
+      <c r="H20">
+        <v>96</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>96</v>
+      </c>
+      <c r="L20">
+        <v>99</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="S20" t="str">
+        <v>A</v>
+      </c>
+      <c r="T20">
+        <v>96</v>
+      </c>
+      <c r="U20">
+        <v>3</v>
+      </c>
+      <c r="V20">
+        <v>6</v>
+      </c>
+      <c r="X20" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y20" s="14">
+        <v>49</v>
+      </c>
+      <c r="Z20" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C21" t="str">
+        <v>B</v>
+      </c>
+      <c r="D21">
+        <v>43</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="G21" t="str">
+        <v>A</v>
+      </c>
+      <c r="H21">
+        <v>99</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <v>99</v>
+      </c>
+      <c r="L21">
+        <v>69</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
+      </c>
+      <c r="S21" t="str">
+        <v>A</v>
+      </c>
+      <c r="T21">
+        <v>99</v>
+      </c>
+      <c r="U21">
+        <v>4</v>
+      </c>
+      <c r="V21">
+        <v>8</v>
+      </c>
+      <c r="X21" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y21" s="14">
+        <v>43</v>
+      </c>
+      <c r="Z21" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C22" t="str">
+        <v>A</v>
+      </c>
+      <c r="D22">
+        <v>96</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="G22" t="str">
+        <v>A</v>
+      </c>
+      <c r="H22">
+        <v>69</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="S22" t="str">
+        <v>A</v>
+      </c>
+      <c r="T22">
+        <v>69</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>9</v>
+      </c>
+      <c r="X22" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y22" s="14">
+        <v>96</v>
+      </c>
+      <c r="Z22" s="14">
+        <v>3</v>
+      </c>
+      <c r="AB22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C23" t="str">
+        <v>B</v>
+      </c>
+      <c r="D23">
+        <v>84</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" t="str">
+        <v>B</v>
+      </c>
+      <c r="T23">
+        <v>49</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>4</v>
+      </c>
+      <c r="X23" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y23" s="14">
+        <v>84</v>
+      </c>
+      <c r="Z23" s="14">
+        <v>2</v>
+      </c>
+      <c r="AB23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C24" t="str">
+        <v>A</v>
+      </c>
+      <c r="D24">
+        <v>99</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="G24" t="str" cm="1">
+        <f t="array" ref="G24:I28">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY($C$17),_xlfn.TAKE(_xlfn.ANCHORARRAY($C$17),,1)=H23)</f>
+        <v>B</v>
+      </c>
+      <c r="H24">
+        <v>49</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="K24" cm="1">
+        <f t="array" ref="K24:K27">_xlfn.DROP(_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(G24),2),-1)</f>
+        <v>49</v>
+      </c>
+      <c r="L24" cm="1">
+        <f t="array" ref="L24:L27">_xlfn.DROP(_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(G24),2),1)</f>
+        <v>43</v>
+      </c>
+      <c r="M24" cm="1">
+        <f t="array" ref="M24:M27">IF(_xlfn.ANCHORARRAY(K24)&gt;_xlfn.ANCHORARRAY(L24),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" cm="1">
+        <f t="array" ref="N24:N27">_xlfn.SCAN(0,_xlfn.ANCHORARRAY(M24),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v=0,1,_xlpm.a+1)))</f>
+        <v>1</v>
+      </c>
+      <c r="P24" cm="1">
+        <f t="array" ref="P24:P28">_xlfn.VSTACK(1,_xlfn.ANCHORARRAY(N24))</f>
+        <v>1</v>
+      </c>
+      <c r="S24" t="str">
+        <v>B</v>
+      </c>
+      <c r="T24">
+        <v>43</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>5</v>
+      </c>
+      <c r="X24" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y24" s="14">
+        <v>99</v>
+      </c>
+      <c r="Z24" s="14">
+        <v>4</v>
+      </c>
+      <c r="AB24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C25" t="str">
+        <v>A</v>
+      </c>
+      <c r="D25">
+        <v>69</v>
+      </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="G25" t="str">
+        <v>B</v>
+      </c>
+      <c r="H25">
+        <v>43</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>43</v>
+      </c>
+      <c r="L25">
+        <v>84</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>2</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="S25" t="str">
+        <v>B</v>
+      </c>
+      <c r="T25">
+        <v>84</v>
+      </c>
+      <c r="U25">
+        <v>2</v>
+      </c>
+      <c r="V25">
+        <v>7</v>
+      </c>
+      <c r="X25" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y25" s="14">
+        <v>69</v>
+      </c>
+      <c r="Z25" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C26" t="str">
+        <v>B</v>
+      </c>
+      <c r="D26">
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="G26" t="str">
+        <v>B</v>
+      </c>
+      <c r="H26">
+        <v>84</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
+      <c r="K26">
+        <v>84</v>
+      </c>
+      <c r="L26">
+        <v>14</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="S26" t="str">
+        <v>B</v>
+      </c>
+      <c r="T26">
+        <v>14</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>10</v>
+      </c>
+      <c r="X26" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y26" s="14">
+        <v>14</v>
+      </c>
+      <c r="Z26" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB26" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC26" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C27" t="str">
+        <v>B</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+      <c r="G27" t="str">
+        <v>B</v>
+      </c>
+      <c r="H27">
+        <v>14</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <v>14</v>
+      </c>
+      <c r="L27">
+        <v>22</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="S27" t="str">
+        <v>B</v>
+      </c>
+      <c r="T27">
+        <v>22</v>
+      </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="V27">
+        <v>11</v>
+      </c>
+      <c r="X27" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y27" s="14">
+        <v>22</v>
+      </c>
+      <c r="Z27" s="14">
+        <v>2</v>
+      </c>
+      <c r="AB27" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC27" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="G28" t="str">
+        <v>B</v>
+      </c>
+      <c r="H28">
+        <v>22</v>
+      </c>
+      <c r="I28">
+        <v>11</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C32" t="str" cm="1">
+        <f t="array" ref="C32:F42" xml:space="preserve"> _xlfn.LET(
+      _xlpm.d, B3:C13,
+      _xlpm.t, _xlfn.HSTACK(_xlpm.d, _xlfn.SEQUENCE(ROWS(_xlpm.d))),
+      _xlpm.u, _xlfn.UNIQUE(_xlfn.TAKE(_xlpm.t, , 1)),
+      _xlpm.v,_xlfn.REDUCE(
+             0,
+             _xlpm.u,
+             _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                    _xlfn.LET(
+                        _xlpm.z,   _xlfn._xlws.FILTER(_xlpm.t, _xlfn.TAKE(_xlpm.t, , 1) = _xlpm.v),
+                        _xlpm.c,   _xlfn.DROP(_xlfn.CHOOSECOLS(_xlpm.z, 2), -1),
+                        _xlpm.c_1, _xlfn.DROP(_xlfn.CHOOSECOLS(_xlpm.z, 2), 1),
+                        _xlpm.zz,  _xlpm.c&gt;_xlpm.c_1,
+                        _xlfn.VSTACK(_xlpm.a,_xlfn.VSTACK(1,_xlfn.SCAN(0,_xlpm.zz,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v=0,1,_xlpm.a+1)))))
+                    )
+             )
+      ),
+     _xlfn.HSTACK(_xlfn._xlws.SORT(_xlpm.t,1),_xlfn.DROP(_xlpm.v,1))
+  )</f>
+        <v>A</v>
+      </c>
+      <c r="D32">
+        <v>100</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" t="str">
+        <v>A</v>
+      </c>
+      <c r="D33">
+        <v>45</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" t="str">
+        <v>A</v>
+      </c>
+      <c r="D34">
+        <v>88</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" t="str">
+        <v>A</v>
+      </c>
+      <c r="D35">
+        <v>96</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" t="str">
+        <v>A</v>
+      </c>
+      <c r="D36" s="1">
+        <v>99</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" t="str">
+        <v>A</v>
+      </c>
+      <c r="D37">
+        <v>69</v>
+      </c>
+      <c r="E37">
+        <v>9</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" t="str">
+        <v>B</v>
+      </c>
+      <c r="D38">
+        <v>49</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" t="str">
+        <v>B</v>
+      </c>
+      <c r="D39">
+        <v>43</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" t="str">
+        <v>B</v>
+      </c>
+      <c r="D40">
+        <v>84</v>
+      </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" t="str">
+        <v>B</v>
+      </c>
+      <c r="D41">
+        <v>14</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" t="str">
+        <v>B</v>
+      </c>
+      <c r="D42">
+        <v>22</v>
+      </c>
+      <c r="E42">
+        <v>11</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Augmented with column headers
</commit_message>
<xml_diff>
--- a/CH-127 Add Index Column.xlsx
+++ b/CH-127 Add Index Column.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7738E7B2-5D36-47BC-A9EC-4AAB619D6B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47C19F7-9D46-4888-9141-BAC60DF34B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -335,10 +335,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -812,15 +812,15 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1079,15 +1079,15 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
@@ -1493,15 +1493,15 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2051,15 +2051,15 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2541,15 +2541,15 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2840,14 +2840,14 @@
       <c r="V17">
         <v>1</v>
       </c>
-      <c r="X17" s="14" t="str" cm="1">
+      <c r="X17" s="13" t="str" cm="1">
         <f t="array" ref="X17:Z27">_xlfn.DROP(_xlfn._xlws.SORT(_xlfn.ANCHORARRAY(S17),4),,-1)</f>
         <v>A</v>
       </c>
-      <c r="Y17" s="14">
+      <c r="Y17" s="13">
         <v>100</v>
       </c>
-      <c r="Z17" s="14">
+      <c r="Z17" s="13">
         <v>1</v>
       </c>
       <c r="AB17" t="b" cm="1">
@@ -2907,13 +2907,13 @@
       <c r="V18">
         <v>2</v>
       </c>
-      <c r="X18" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y18" s="14">
+      <c r="X18" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y18" s="13">
         <v>45</v>
       </c>
-      <c r="Z18" s="14">
+      <c r="Z18" s="13">
         <v>1</v>
       </c>
       <c r="AB18" t="b">
@@ -2972,13 +2972,13 @@
       <c r="V19">
         <v>3</v>
       </c>
-      <c r="X19" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y19" s="14">
+      <c r="X19" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y19" s="13">
         <v>88</v>
       </c>
-      <c r="Z19" s="14">
+      <c r="Z19" s="13">
         <v>2</v>
       </c>
       <c r="AB19" t="b">
@@ -3037,13 +3037,13 @@
       <c r="V20">
         <v>6</v>
       </c>
-      <c r="X20" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y20" s="14">
+      <c r="X20" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y20" s="13">
         <v>49</v>
       </c>
-      <c r="Z20" s="14">
+      <c r="Z20" s="13">
         <v>1</v>
       </c>
       <c r="AB20" t="b">
@@ -3102,13 +3102,13 @@
       <c r="V21">
         <v>8</v>
       </c>
-      <c r="X21" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y21" s="14">
+      <c r="X21" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y21" s="13">
         <v>43</v>
       </c>
-      <c r="Z21" s="14">
+      <c r="Z21" s="13">
         <v>1</v>
       </c>
       <c r="AB21" t="b">
@@ -3155,13 +3155,13 @@
       <c r="V22">
         <v>9</v>
       </c>
-      <c r="X22" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y22" s="14">
+      <c r="X22" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y22" s="13">
         <v>96</v>
       </c>
-      <c r="Z22" s="14">
+      <c r="Z22" s="13">
         <v>3</v>
       </c>
       <c r="AB22" t="b">
@@ -3205,13 +3205,13 @@
       <c r="V23">
         <v>4</v>
       </c>
-      <c r="X23" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y23" s="14">
+      <c r="X23" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y23" s="13">
         <v>84</v>
       </c>
-      <c r="Z23" s="14">
+      <c r="Z23" s="13">
         <v>2</v>
       </c>
       <c r="AB23" t="b">
@@ -3276,13 +3276,13 @@
       <c r="V24">
         <v>5</v>
       </c>
-      <c r="X24" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y24" s="14">
+      <c r="X24" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y24" s="13">
         <v>99</v>
       </c>
-      <c r="Z24" s="14">
+      <c r="Z24" s="13">
         <v>4</v>
       </c>
       <c r="AB24" t="b">
@@ -3341,13 +3341,13 @@
       <c r="V25">
         <v>7</v>
       </c>
-      <c r="X25" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y25" s="14">
+      <c r="X25" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y25" s="13">
         <v>69</v>
       </c>
-      <c r="Z25" s="14">
+      <c r="Z25" s="13">
         <v>1</v>
       </c>
       <c r="AB25" t="b">
@@ -3406,13 +3406,13 @@
       <c r="V26">
         <v>10</v>
       </c>
-      <c r="X26" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y26" s="14">
+      <c r="X26" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y26" s="13">
         <v>14</v>
       </c>
-      <c r="Z26" s="14">
+      <c r="Z26" s="13">
         <v>1</v>
       </c>
       <c r="AB26" t="b">
@@ -3471,13 +3471,13 @@
       <c r="V27">
         <v>11</v>
       </c>
-      <c r="X27" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y27" s="14">
+      <c r="X27" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y27" s="13">
         <v>22</v>
       </c>
-      <c r="Z27" s="14">
+      <c r="Z27" s="13">
         <v>2</v>
       </c>
       <c r="AB27" t="b">
@@ -3519,10 +3519,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0759260A-3526-4E7B-9B81-CFE36C329450}">
-  <dimension ref="A1:AD42"/>
+  <dimension ref="A1:AD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L33" sqref="L32:L33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3536,15 +3536,15 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
@@ -3961,14 +3961,14 @@
       <c r="V17">
         <v>1</v>
       </c>
-      <c r="X17" s="14" t="str" cm="1">
+      <c r="X17" s="13" t="str" cm="1">
         <f t="array" ref="X17:Z27">_xlfn.DROP(_xlfn._xlws.SORT(_xlfn.ANCHORARRAY(S17),4),,-1)</f>
         <v>A</v>
       </c>
-      <c r="Y17" s="14">
+      <c r="Y17" s="13">
         <v>100</v>
       </c>
-      <c r="Z17" s="14">
+      <c r="Z17" s="13">
         <v>1</v>
       </c>
       <c r="AB17" t="b" cm="1">
@@ -4028,13 +4028,13 @@
       <c r="V18">
         <v>2</v>
       </c>
-      <c r="X18" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y18" s="14">
+      <c r="X18" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y18" s="13">
         <v>45</v>
       </c>
-      <c r="Z18" s="14">
+      <c r="Z18" s="13">
         <v>1</v>
       </c>
       <c r="AB18" t="b">
@@ -4093,13 +4093,13 @@
       <c r="V19">
         <v>3</v>
       </c>
-      <c r="X19" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y19" s="14">
+      <c r="X19" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y19" s="13">
         <v>88</v>
       </c>
-      <c r="Z19" s="14">
+      <c r="Z19" s="13">
         <v>2</v>
       </c>
       <c r="AB19" t="b">
@@ -4158,13 +4158,13 @@
       <c r="V20">
         <v>6</v>
       </c>
-      <c r="X20" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y20" s="14">
+      <c r="X20" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y20" s="13">
         <v>49</v>
       </c>
-      <c r="Z20" s="14">
+      <c r="Z20" s="13">
         <v>1</v>
       </c>
       <c r="AB20" t="b">
@@ -4223,13 +4223,13 @@
       <c r="V21">
         <v>8</v>
       </c>
-      <c r="X21" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y21" s="14">
+      <c r="X21" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y21" s="13">
         <v>43</v>
       </c>
-      <c r="Z21" s="14">
+      <c r="Z21" s="13">
         <v>1</v>
       </c>
       <c r="AB21" t="b">
@@ -4276,13 +4276,13 @@
       <c r="V22">
         <v>9</v>
       </c>
-      <c r="X22" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y22" s="14">
+      <c r="X22" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y22" s="13">
         <v>96</v>
       </c>
-      <c r="Z22" s="14">
+      <c r="Z22" s="13">
         <v>3</v>
       </c>
       <c r="AB22" t="b">
@@ -4326,13 +4326,13 @@
       <c r="V23">
         <v>4</v>
       </c>
-      <c r="X23" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y23" s="14">
+      <c r="X23" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y23" s="13">
         <v>84</v>
       </c>
-      <c r="Z23" s="14">
+      <c r="Z23" s="13">
         <v>2</v>
       </c>
       <c r="AB23" t="b">
@@ -4397,13 +4397,13 @@
       <c r="V24">
         <v>5</v>
       </c>
-      <c r="X24" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y24" s="14">
+      <c r="X24" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y24" s="13">
         <v>99</v>
       </c>
-      <c r="Z24" s="14">
+      <c r="Z24" s="13">
         <v>4</v>
       </c>
       <c r="AB24" t="b">
@@ -4462,13 +4462,13 @@
       <c r="V25">
         <v>7</v>
       </c>
-      <c r="X25" s="14" t="str">
-        <v>A</v>
-      </c>
-      <c r="Y25" s="14">
+      <c r="X25" s="13" t="str">
+        <v>A</v>
+      </c>
+      <c r="Y25" s="13">
         <v>69</v>
       </c>
-      <c r="Z25" s="14">
+      <c r="Z25" s="13">
         <v>1</v>
       </c>
       <c r="AB25" t="b">
@@ -4527,13 +4527,13 @@
       <c r="V26">
         <v>10</v>
       </c>
-      <c r="X26" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y26" s="14">
+      <c r="X26" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y26" s="13">
         <v>14</v>
       </c>
-      <c r="Z26" s="14">
+      <c r="Z26" s="13">
         <v>1</v>
       </c>
       <c r="AB26" t="b">
@@ -4592,13 +4592,13 @@
       <c r="V27">
         <v>11</v>
       </c>
-      <c r="X27" s="14" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y27" s="14">
+      <c r="X27" s="13" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y27" s="13">
         <v>22</v>
       </c>
-      <c r="Z27" s="14">
+      <c r="Z27" s="13">
         <v>2</v>
       </c>
       <c r="AB27" t="b">
@@ -4626,8 +4626,8 @@
       </c>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="C32" t="str" cm="1">
-        <f t="array" ref="C32:E42" xml:space="preserve"> _xlfn.LET(
+      <c r="C32" s="4" t="str" cm="1">
+        <f t="array" ref="C32:E43" xml:space="preserve"> _xlfn.LET(
       _xlpm.d, B3:C13,
       _xlpm.t, _xlfn.HSTACK(_xlpm.d, _xlfn.SEQUENCE(ROWS(_xlpm.d))),
       _xlpm.u, _xlfn.UNIQUE(_xlfn.TAKE(_xlpm.t, , 1)),
@@ -4643,223 +4643,243 @@
                         _xlfn.VSTACK(_xlpm.a,_xlfn.VSTACK(1,_xlfn.SCAN(0,_xlpm.zz,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v=0,1,_xlpm.a+1)))))
                     )
              )
-      ),_xlfn.CHOOSECOLS(_xlfn._xlws.SORT(_xlfn.HSTACK(_xlfn._xlws.SORT(_xlpm.t,1),_xlfn.DROP(_xlpm.v_1,1)),3),1,2,4))</f>
-        <v>A</v>
-      </c>
-      <c r="D32">
+      ),_xlfn.VSTACK(E2:G2,_xlfn.CHOOSECOLS(_xlfn._xlws.SORT(_xlfn.HSTACK(_xlfn._xlws.SORT(_xlpm.t,1),_xlfn.DROP(_xlpm.v_1,1)),3),1,2,4)))</f>
+        <v>Stock</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <v>Price</v>
+      </c>
+      <c r="E32" s="6" t="str">
+        <v>index</v>
+      </c>
+      <c r="G32" t="b" cm="1">
+        <f t="array" ref="G32:I43">_xlfn.ANCHORARRAY(C32)=E2:G13</f>
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="D33" s="9">
         <v>100</v>
       </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="b" cm="1">
-        <f t="array" ref="G32:I42">_xlfn.ANCHORARRAY(C32)=E3:G13</f>
-        <v>1</v>
-      </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C33" t="str">
-        <v>A</v>
-      </c>
-      <c r="D33">
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C34" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="D34" s="9">
         <v>45</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C34" t="str">
-        <v>A</v>
-      </c>
-      <c r="D34">
+      <c r="E34" s="7">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C35" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="D35" s="9">
         <v>88</v>
       </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="G34" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C35" t="str">
-        <v>B</v>
-      </c>
-      <c r="D35">
+      <c r="E35" s="7">
+        <v>2</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C36" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="D36" s="9">
         <v>49</v>
       </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C36" t="str">
-        <v>B</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="E36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C37" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="D37" s="9">
         <v>43</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" t="str">
-        <v>A</v>
-      </c>
-      <c r="D37">
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="D38" s="9">
         <v>96</v>
       </c>
-      <c r="E37">
-        <v>3</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C38" t="str">
-        <v>B</v>
-      </c>
-      <c r="D38">
+      <c r="E38" s="7">
+        <v>3</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="D39" s="9">
         <v>84</v>
       </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C39" t="str">
-        <v>A</v>
-      </c>
-      <c r="D39">
+      <c r="E39" s="7">
+        <v>2</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="D40" s="9">
         <v>99</v>
       </c>
-      <c r="E39">
-        <v>4</v>
-      </c>
-      <c r="G39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C40" t="str">
-        <v>A</v>
-      </c>
-      <c r="D40">
+      <c r="E40" s="7">
+        <v>4</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="D41" s="9">
         <v>69</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="G40" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C41" t="str">
-        <v>B</v>
-      </c>
-      <c r="D41">
+      <c r="E41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="D42" s="9">
         <v>14</v>
       </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="G41" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C42" t="str">
-        <v>B</v>
-      </c>
-      <c r="D42">
+      <c r="E42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="D43" s="9">
         <v>22</v>
       </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
-      <c r="G42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" t="b">
+      <c r="E43" s="7">
+        <v>2</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>